<commit_message>
Mises à jour des fichiers binaires et suppression des fichiers d'images
</commit_message>
<xml_diff>
--- a/Livrables/Livrable_10_Rapport_de_management/Samuel/Liste_des_tâches_pour_le_projet_SAE.xlsx
+++ b/Livrables/Livrable_10_Rapport_de_management/Samuel/Liste_des_tâches_pour_le_projet_SAE.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="76">
   <si>
     <t>Liste des tâches pour le projet SAE</t>
   </si>
@@ -85,6 +85,15 @@
     <t>Back-end</t>
   </si>
   <si>
+    <t>Création d'un dépôt de code sur Hugging Face</t>
+  </si>
+  <si>
+    <t>Alexandre</t>
+  </si>
+  <si>
+    <t>Back-end &amp; Production</t>
+  </si>
+  <si>
     <t>Analyse des conditions juridiques d'utilisation des données</t>
   </si>
   <si>
@@ -94,10 +103,7 @@
     <t>Analyse des conditions juridiques d'utilisation des jeux de données</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Alexandre</t>
+    <t>Aurélien</t>
   </si>
   <si>
     <t>Prise en main de GPT-2 et tests avec Jupyter Notebook et TensorFlow/Keras</t>
@@ -112,13 +118,10 @@
     <t>Alexandre &amp; Lucas</t>
   </si>
   <si>
-    <t>Aurélien</t>
+    <t>Quentin</t>
   </si>
   <si>
     <t>Utilisation de l'API TensorFlow pour interroger le modèle pré-entraîné</t>
-  </si>
-  <si>
-    <t>Quentin</t>
   </si>
   <si>
     <t>Tests avec Jupyter Notebook et TensorFlow/Keras</t>
@@ -148,7 +151,7 @@
     <t>Fine-tuning du modèle GPT-2 avec l'ensemble de données de dialogue</t>
   </si>
   <si>
-    <t>Ony &amp; Quentin</t>
+    <t>Samuel, Alexandre &amp; Quentin</t>
   </si>
   <si>
     <t>Optimisation du modèle pour la génération de réponses cohérentes et pertinentes</t>
@@ -160,7 +163,10 @@
     <t>Utilisation de la bibliothèque Gradio pour créer une interface utilisateur</t>
   </si>
   <si>
-    <t>Ony &amp; Samuel</t>
+    <t>Ony &amp; Aurelien</t>
+  </si>
+  <si>
+    <t>Production d'une maquette avec figma</t>
   </si>
   <si>
     <t>Personnalisation de l'interface utilisateur</t>
@@ -175,7 +181,7 @@
     <t>Évaluation des performances du modèle fine-tuné</t>
   </si>
   <si>
-    <t>Lucas, Quentin, Aurelien &amp; Alexandre</t>
+    <t>Lucas, Quentin &amp; Alexandre</t>
   </si>
   <si>
     <t>Comparaison entre le modèle générique et le modèle spécialisé</t>
@@ -184,16 +190,25 @@
     <t>Rédaction d'un rapport sur les résultats</t>
   </si>
   <si>
-    <t>Optimisation du modèle Fine-tuning</t>
+    <t xml:space="preserve">Optimisation </t>
+  </si>
+  <si>
+    <t>Optimisation du modèle Fine-tuning et Gradio</t>
   </si>
   <si>
     <t>Analyse des retours utilisateurs</t>
   </si>
   <si>
+    <t>Ony &amp; Aurélien</t>
+  </si>
+  <si>
     <t>Ajustements du modèle en fonction des retours</t>
   </si>
   <si>
-    <t>Optimisation des performances du modèle</t>
+    <t>Optimisation</t>
+  </si>
+  <si>
+    <t>Ony &amp; Quentin &amp; Alexandre</t>
   </si>
   <si>
     <t>Rapports individuels sur le travail réalisé</t>
@@ -205,7 +220,7 @@
     <t>Rédaction d'un rapport individuel sur le travail réalisé pendant chaque période de deux semaines</t>
   </si>
   <si>
-    <t>All</t>
+    <t>Tous</t>
   </si>
   <si>
     <t>Rapports de management détaillant la répartition et la planification des tâches</t>
@@ -242,7 +257,7 @@
     </font>
     <font>
       <b/>
-      <sz val="16.0"/>
+      <sz val="22.0"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -398,10 +413,7 @@
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -414,6 +426,9 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -430,8 +445,8 @@
     <xf borderId="4" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -761,35 +776,35 @@
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="O3" s="4"/>
@@ -810,25 +825,25 @@
       <c r="AD3" s="4"/>
     </row>
     <row r="4" ht="37.5" customHeight="1">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>1.0</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>45219.0</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>15</v>
       </c>
       <c r="H4" s="11" t="s">
@@ -838,10 +853,10 @@
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="N4" s="10" t="s">
         <v>17</v>
       </c>
       <c r="O4" s="12"/>
@@ -867,10 +882,10 @@
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="10" t="s">
         <v>15</v>
       </c>
       <c r="H5" s="11" t="s">
@@ -880,7 +895,7 @@
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
-      <c r="M5" s="11" t="s">
+      <c r="M5" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N5" s="14" t="s">
@@ -904,16 +919,16 @@
       <c r="AD5" s="12"/>
     </row>
     <row r="6" ht="37.5" customHeight="1">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="11" t="s">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>15</v>
+      <c r="G6" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>16</v>
@@ -922,7 +937,7 @@
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
-      <c r="M6" s="11" t="s">
+      <c r="M6" s="10" t="s">
         <v>22</v>
       </c>
       <c r="N6" s="14" t="s">
@@ -946,40 +961,29 @@
       <c r="AD6" s="12"/>
     </row>
     <row r="7" ht="37.5" customHeight="1">
-      <c r="A7" s="16">
-        <f>A4+1</f>
-        <v>2</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="17">
-        <v>45247.0</v>
-      </c>
-      <c r="D7" s="11" t="s">
+      <c r="G7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>15</v>
-      </c>
       <c r="H7" s="11" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
-      <c r="M7" s="11" t="s">
-        <v>28</v>
+      <c r="M7" s="10" t="s">
+        <v>25</v>
       </c>
-      <c r="N7" s="11" t="s">
-        <v>23</v>
+      <c r="N7" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
@@ -999,37 +1003,39 @@
       <c r="AD7" s="12"/>
     </row>
     <row r="8" ht="37.5" customHeight="1">
-      <c r="A8" s="8">
-        <f>A7+1</f>
-        <v>3</v>
+      <c r="A8" s="16">
+        <f>A4+1</f>
+        <v>2</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="17">
+        <v>45247.0</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="10">
-        <v>45247.0</v>
+      <c r="G8" s="10" t="s">
+        <v>15</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>12</v>
+      <c r="H8" s="11" t="s">
+        <v>16</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="18"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
-      <c r="M8" s="11" t="s">
-        <v>33</v>
+      <c r="M8" s="10" t="s">
+        <v>30</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="N8" s="10" t="s">
         <v>23</v>
       </c>
       <c r="O8" s="12"/>
@@ -1050,23 +1056,36 @@
       <c r="AD8" s="12"/>
     </row>
     <row r="9" ht="37.5" customHeight="1">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="11" t="s">
+      <c r="A9" s="7">
+        <f>A8+1</f>
+        <v>3</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="9">
+        <v>45247.0</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>32</v>
+      <c r="H9" s="11" t="s">
+        <v>16</v>
       </c>
-      <c r="H9" s="18"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
-      <c r="M9" s="11" t="s">
+      <c r="M9" s="10" t="s">
         <v>35</v>
       </c>
       <c r="N9" s="14" t="s">
@@ -1090,24 +1109,24 @@
       <c r="AD9" s="12"/>
     </row>
     <row r="10" ht="37.5" customHeight="1">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="11" t="s">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>32</v>
+      <c r="G10" s="10" t="s">
+        <v>34</v>
       </c>
-      <c r="H10" s="18"/>
+      <c r="H10" s="11" t="s">
+        <v>16</v>
+      </c>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
@@ -1126,29 +1145,20 @@
       <c r="AD10" s="12"/>
     </row>
     <row r="11" ht="37.5" customHeight="1">
-      <c r="A11" s="8">
-        <f>A8+1</f>
-        <v>4</v>
-      </c>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="10">
-        <v>45278.0</v>
+      <c r="G11" s="10" t="s">
+        <v>34</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>12</v>
+      <c r="H11" s="11" t="s">
+        <v>16</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="18"/>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
@@ -1173,18 +1183,31 @@
       <c r="AD11" s="12"/>
     </row>
     <row r="12" ht="37.5" customHeight="1">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="11" t="s">
+      <c r="A12" s="7">
+        <f>A9+1</f>
+        <v>4</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="9">
+        <v>45278.0</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="11" t="s">
-        <v>40</v>
+      <c r="H12" s="11" t="s">
+        <v>16</v>
       </c>
-      <c r="H12" s="18"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
@@ -1209,18 +1232,20 @@
       <c r="AD12" s="12"/>
     </row>
     <row r="13" ht="37.5" customHeight="1">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="11" t="s">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>40</v>
+      <c r="G13" s="10" t="s">
+        <v>41</v>
       </c>
-      <c r="H13" s="18"/>
+      <c r="H13" s="11" t="s">
+        <v>16</v>
+      </c>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
@@ -1245,29 +1270,20 @@
       <c r="AD13" s="12"/>
     </row>
     <row r="14" ht="37.5" customHeight="1">
-      <c r="A14" s="8">
-        <f>A11+1</f>
-        <v>5</v>
-      </c>
-      <c r="B14" s="9" t="s">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="10">
-        <v>44945.0</v>
+      <c r="G14" s="10" t="s">
+        <v>41</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>12</v>
+      <c r="H14" s="11" t="s">
+        <v>16</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="18"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
@@ -1292,18 +1308,31 @@
       <c r="AD14" s="12"/>
     </row>
     <row r="15" ht="37.5" customHeight="1">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="11" t="s">
+      <c r="A15" s="7">
+        <f>A12+1</f>
+        <v>5</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="9">
+        <v>45310.0</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="11" t="s">
-        <v>45</v>
+      <c r="H15" s="11" t="s">
+        <v>16</v>
       </c>
-      <c r="H15" s="18"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
@@ -1328,29 +1357,20 @@
       <c r="AD15" s="12"/>
     </row>
     <row r="16" ht="37.5" customHeight="1">
-      <c r="A16" s="8">
-        <f>A14+1</f>
-        <v>6</v>
-      </c>
-      <c r="B16" s="9" t="s">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="10">
-        <v>44945.0</v>
+      <c r="G16" s="10" t="s">
+        <v>46</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>12</v>
+      <c r="H16" s="11" t="s">
+        <v>16</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="18"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
@@ -1375,18 +1395,31 @@
       <c r="AD16" s="12"/>
     </row>
     <row r="17" ht="37.5" customHeight="1">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="11" t="s">
+      <c r="A17" s="7">
+        <f>A15+1</f>
+        <v>6</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="9">
+        <v>45310.0</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G17" s="11" t="s">
-        <v>49</v>
+      <c r="H17" s="11" t="s">
+        <v>16</v>
       </c>
-      <c r="H17" s="18"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
@@ -1411,29 +1444,20 @@
       <c r="AD17" s="12"/>
     </row>
     <row r="18" ht="37.5" customHeight="1">
-      <c r="A18" s="8">
-        <f>A16+1</f>
-        <v>7</v>
-      </c>
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="10">
-        <v>45338.0</v>
+      <c r="G18" s="10" t="s">
+        <v>19</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>12</v>
+      <c r="H18" s="11" t="s">
+        <v>16</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="H18" s="18"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
@@ -1458,18 +1482,20 @@
       <c r="AD18" s="12"/>
     </row>
     <row r="19" ht="37.5" customHeight="1">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="11" t="s">
-        <v>55</v>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="10" t="s">
+        <v>52</v>
       </c>
-      <c r="G19" s="11" t="s">
-        <v>54</v>
+      <c r="G19" s="10" t="s">
+        <v>19</v>
       </c>
-      <c r="H19" s="18"/>
+      <c r="H19" s="11" t="s">
+        <v>16</v>
+      </c>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
@@ -1494,18 +1520,31 @@
       <c r="AD19" s="12"/>
     </row>
     <row r="20" ht="37.5" customHeight="1">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="11" t="s">
+      <c r="A20" s="7">
+        <f>A17+1</f>
+        <v>7</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="9">
+        <v>45338.0</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="G20" s="11" t="s">
-        <v>54</v>
+      <c r="H20" s="11" t="s">
+        <v>16</v>
       </c>
-      <c r="H20" s="18"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
@@ -1530,29 +1569,20 @@
       <c r="AD20" s="12"/>
     </row>
     <row r="21" ht="37.5" customHeight="1">
-      <c r="A21" s="8">
-        <f>A18+1</f>
-        <v>8</v>
-      </c>
-      <c r="B21" s="9" t="s">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="10">
-        <v>45355.0</v>
+      <c r="G21" s="10" t="s">
+        <v>56</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>12</v>
+      <c r="H21" s="11" t="s">
+        <v>16</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H21" s="18"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
@@ -1577,18 +1607,20 @@
       <c r="AD21" s="12"/>
     </row>
     <row r="22" ht="37.5" customHeight="1">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="11" t="s">
-        <v>59</v>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="10" t="s">
+        <v>58</v>
       </c>
-      <c r="G22" s="11" t="s">
-        <v>45</v>
+      <c r="G22" s="10" t="s">
+        <v>56</v>
       </c>
-      <c r="H22" s="18"/>
+      <c r="H22" s="11" t="s">
+        <v>16</v>
+      </c>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
@@ -1613,18 +1645,31 @@
       <c r="AD22" s="12"/>
     </row>
     <row r="23" ht="37.5" customHeight="1">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="11" t="s">
+      <c r="A23" s="7">
+        <f>A20+1</f>
+        <v>8</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="9">
+        <v>45355.0</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G23" s="11" t="s">
-        <v>45</v>
+      <c r="F23" s="10" t="s">
+        <v>61</v>
       </c>
-      <c r="H23" s="18"/>
+      <c r="G23" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>16</v>
+      </c>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
@@ -1649,29 +1694,20 @@
       <c r="AD23" s="12"/>
     </row>
     <row r="24" ht="37.5" customHeight="1">
-      <c r="A24" s="16">
-        <f>A21+1</f>
-        <v>9</v>
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="10" t="s">
+        <v>63</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="11" t="s">
+      <c r="G24" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>25</v>
+      <c r="H24" s="11" t="s">
+        <v>16</v>
       </c>
-      <c r="E24" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="H24" s="18"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
@@ -1696,29 +1732,20 @@
       <c r="AD24" s="12"/>
     </row>
     <row r="25" ht="37.5" customHeight="1">
-      <c r="A25" s="8">
-        <f>A24+1</f>
-        <v>10</v>
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="10" t="s">
+        <v>64</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="G25" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>62</v>
+      <c r="H25" s="11" t="s">
+        <v>16</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H25" s="18"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
@@ -1743,18 +1770,31 @@
       <c r="AD25" s="12"/>
     </row>
     <row r="26" ht="37.5" customHeight="1">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="11" t="s">
+      <c r="A26" s="16">
+        <f>A23+1</f>
+        <v>9</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="G26" s="11" t="s">
-        <v>64</v>
+      <c r="H26" s="11" t="s">
+        <v>16</v>
       </c>
-      <c r="H26" s="18"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
@@ -1779,18 +1819,31 @@
       <c r="AD26" s="12"/>
     </row>
     <row r="27" ht="37.5" customHeight="1">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="11" t="s">
+      <c r="A27" s="7">
+        <f>A26+1</f>
+        <v>10</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G27" s="11" t="s">
-        <v>68</v>
+      <c r="C27" s="8" t="s">
+        <v>67</v>
       </c>
-      <c r="H27" s="18"/>
+      <c r="D27" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>16</v>
+      </c>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
@@ -1814,69 +1867,81 @@
       <c r="AC27" s="12"/>
       <c r="AD27" s="12"/>
     </row>
-    <row r="28">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="4"/>
-      <c r="Y28" s="4"/>
-      <c r="Z28" s="4"/>
-      <c r="AA28" s="4"/>
-      <c r="AB28" s="4"/>
-      <c r="AC28" s="4"/>
-      <c r="AD28" s="4"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
-      <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
-      <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
-      <c r="Z29" s="4"/>
-      <c r="AA29" s="4"/>
-      <c r="AB29" s="4"/>
-      <c r="AC29" s="4"/>
-      <c r="AD29" s="4"/>
+    <row r="28" ht="37.5" customHeight="1">
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="12"/>
+      <c r="U28" s="12"/>
+      <c r="V28" s="12"/>
+      <c r="W28" s="12"/>
+      <c r="X28" s="12"/>
+      <c r="Y28" s="12"/>
+      <c r="Z28" s="12"/>
+      <c r="AA28" s="12"/>
+      <c r="AB28" s="12"/>
+      <c r="AC28" s="12"/>
+      <c r="AD28" s="12"/>
+    </row>
+    <row r="29" ht="37.5" customHeight="1">
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="12"/>
+      <c r="U29" s="12"/>
+      <c r="V29" s="12"/>
+      <c r="W29" s="12"/>
+      <c r="X29" s="12"/>
+      <c r="Y29" s="12"/>
+      <c r="Z29" s="12"/>
+      <c r="AA29" s="12"/>
+      <c r="AB29" s="12"/>
+      <c r="AC29" s="12"/>
+      <c r="AD29" s="12"/>
     </row>
     <row r="30">
       <c r="A30" s="4"/>
@@ -33334,69 +33399,133 @@
       <c r="AC1012" s="4"/>
       <c r="AD1012" s="4"/>
     </row>
+    <row r="1013">
+      <c r="A1013" s="4"/>
+      <c r="B1013" s="4"/>
+      <c r="C1013" s="4"/>
+      <c r="D1013" s="4"/>
+      <c r="E1013" s="4"/>
+      <c r="F1013" s="4"/>
+      <c r="G1013" s="4"/>
+      <c r="H1013" s="4"/>
+      <c r="I1013" s="4"/>
+      <c r="J1013" s="4"/>
+      <c r="K1013" s="4"/>
+      <c r="L1013" s="4"/>
+      <c r="M1013" s="4"/>
+      <c r="N1013" s="4"/>
+      <c r="O1013" s="4"/>
+      <c r="P1013" s="4"/>
+      <c r="Q1013" s="4"/>
+      <c r="R1013" s="4"/>
+      <c r="S1013" s="4"/>
+      <c r="T1013" s="4"/>
+      <c r="U1013" s="4"/>
+      <c r="V1013" s="4"/>
+      <c r="W1013" s="4"/>
+      <c r="X1013" s="4"/>
+      <c r="Y1013" s="4"/>
+      <c r="Z1013" s="4"/>
+      <c r="AA1013" s="4"/>
+      <c r="AB1013" s="4"/>
+      <c r="AC1013" s="4"/>
+      <c r="AD1013" s="4"/>
+    </row>
+    <row r="1014">
+      <c r="A1014" s="4"/>
+      <c r="B1014" s="4"/>
+      <c r="C1014" s="4"/>
+      <c r="D1014" s="4"/>
+      <c r="E1014" s="4"/>
+      <c r="F1014" s="4"/>
+      <c r="G1014" s="4"/>
+      <c r="H1014" s="4"/>
+      <c r="I1014" s="4"/>
+      <c r="J1014" s="4"/>
+      <c r="K1014" s="4"/>
+      <c r="L1014" s="4"/>
+      <c r="M1014" s="4"/>
+      <c r="N1014" s="4"/>
+      <c r="O1014" s="4"/>
+      <c r="P1014" s="4"/>
+      <c r="Q1014" s="4"/>
+      <c r="R1014" s="4"/>
+      <c r="S1014" s="4"/>
+      <c r="T1014" s="4"/>
+      <c r="U1014" s="4"/>
+      <c r="V1014" s="4"/>
+      <c r="W1014" s="4"/>
+      <c r="X1014" s="4"/>
+      <c r="Y1014" s="4"/>
+      <c r="Z1014" s="4"/>
+      <c r="AA1014" s="4"/>
+      <c r="AB1014" s="4"/>
+      <c r="AC1014" s="4"/>
+      <c r="AD1014" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="42">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
   </mergeCells>
-  <conditionalFormatting sqref="H4:H27">
+  <conditionalFormatting sqref="H4:H29">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"V"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
+  <conditionalFormatting sqref="H8">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
+  <conditionalFormatting sqref="H8">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="portrait" pageOrder="overThenDown"/>
+  <pageSetup fitToWidth="0" paperSize="8" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>